<commit_message>
Update Book Ten 2nd Half 50 - 60.xlsx
</commit_message>
<xml_diff>
--- a/content/Book Ten 2nd Half 50 - 60.xlsx
+++ b/content/Book Ten 2nd Half 50 - 60.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5A6752-CC06-4849-84E4-11712AB63527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F210B5-88CC-4CF0-A7C9-A489118DD6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="923" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20848,8 +20848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D440" sqref="D440"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="92" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20910,6 +20910,12 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6799</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>

</xml_diff>